<commit_message>
fix: streamline image upload handling and improve temporary file management
</commit_message>
<xml_diff>
--- a/static/doc/excel/data_admin_sub_admin.xlsx
+++ b/static/doc/excel/data_admin_sub_admin.xlsx
@@ -152,6 +152,106 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>4</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>5</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>6</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="476250" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -444,7 +544,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -453,10 +553,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
     <col width="4" customWidth="1" style="1" min="1" max="1"/>
-    <col width="8" customWidth="1" style="1" min="2" max="2"/>
-    <col width="17" customWidth="1" style="1" min="3" max="3"/>
+    <col width="32" customWidth="1" style="1" min="2" max="2"/>
+    <col width="18" customWidth="1" style="1" min="3" max="3"/>
     <col width="13" customWidth="1" style="1" min="4" max="4"/>
-    <col width="7" customWidth="1" style="1" min="5" max="5"/>
+    <col width="11" customWidth="1" style="1" min="5" max="5"/>
     <col width="13" customWidth="1" style="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -505,7 +605,7 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Admin1</t>
+          <t>Administrator Superuser</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
@@ -525,7 +625,127 @@
       </c>
       <c r="F3" s="5" t="inlineStr">
         <is>
-          <t>https://i.ibb.co.com/k4cwRSL/forgot-password-concept-illustration.png forgot-password-concept-illustration.png</t>
+          <t>https://i.ibb.co.com/qYvWbwVj/unnamed.jpg unnamed.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="44" customHeight="1">
+      <c r="A4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Salahudin Kholik Prasetonosa</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>admin1@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>Superuser</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co.com/B2FVd2n6/ui-design.png ui-design.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="44" customHeight="1">
+      <c r="A5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>taufiqs</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>admin4@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Mentor</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co.com/5Yd94zx/user.png user.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="44" customHeight="1">
+      <c r="A6" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Salahudin kholik Prasetyono</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>admin5@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>Mentor</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Sub Admin</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co.com/5Yd94zx/user.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="44" customHeight="1">
+      <c r="A7" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Salahudin Kholik Prasetyonobos</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="inlineStr">
+        <is>
+          <t>admin2@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="inlineStr">
+        <is>
+          <t>Superuser</t>
+        </is>
+      </c>
+      <c r="E7" s="4" t="inlineStr">
+        <is>
+          <t>Sub Admin</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>https://i.ibb.co.com/5Yd94zx/user.png</t>
         </is>
       </c>
     </row>

</xml_diff>